<commit_message>
added Spoting and KMFL data
</commit_message>
<xml_diff>
--- a/PalladiumDwh.ClientReader.Infrastructure/Seed/Validator.xlsx
+++ b/PalladiumDwh.ClientReader.Infrastructure/Seed/Validator.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4455"/>
   </bookViews>
   <sheets>
     <sheet name="Validator" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="163">
   <si>
     <t>Id</t>
   </si>
@@ -39,166 +39,475 @@
     <t>Summary</t>
   </si>
   <si>
+    <t>61bbda3e-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>TempPatientArtExtract</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>Logical</t>
+  </si>
+  <si>
+    <t>DOB &gt;= LastVisit AND LastVisit IS NOT NULL</t>
+  </si>
+  <si>
+    <t>DoB After LastVisit</t>
+  </si>
+  <si>
+    <t>61bbe4f2-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>DOB &gt; = PreviousARTStartDate AND PreviousARTStartDate IS NOT NULL</t>
+  </si>
+  <si>
+    <t>DOB after PreviousARTStartDate</t>
+  </si>
+  <si>
+    <t>61bbed08-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>DOB &gt; StartARTDate</t>
+  </si>
+  <si>
+    <t>DOB greater than StartARTDate</t>
+  </si>
+  <si>
+    <t>61bbf0a0-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>DOB &gt;=ExitDate AND ExitDate IS NOT NULL</t>
+  </si>
+  <si>
+    <t>DoB After ExitDate</t>
+  </si>
+  <si>
+    <t>61bc2d9a-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>DOB &gt;=ExpectedReturn AND ExpectedReturn IS NOT NULL</t>
+  </si>
+  <si>
+    <t>DoB After ExpectedReturn</t>
+  </si>
+  <si>
+    <t>61bbd912-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>ExitReason</t>
+  </si>
+  <si>
+    <t>ExitReason IS NULL AND ExitDate IS NOT NULL</t>
+  </si>
+  <si>
+    <t>Missing Exit Reason</t>
+  </si>
+  <si>
+    <t>61bc219c-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>ExpectedReturn</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>ExpectedReturn IS NULL</t>
+  </si>
+  <si>
+    <t>ExpectedReturn is Required</t>
+  </si>
+  <si>
+    <t>61bc32fe-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>LastRegimen</t>
+  </si>
+  <si>
+    <t>LastARTDate IS NOT NULL AND LastRegimen IS NULL</t>
+  </si>
+  <si>
+    <t>LastRegimen details missing</t>
+  </si>
+  <si>
+    <t>61bbe1be-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>LastRegimenLine</t>
+  </si>
+  <si>
+    <t>LastARTDate IS NOT NULL AND LastRegimenLine IS NULL</t>
+  </si>
+  <si>
+    <t>LastRegimenLine details missing</t>
+  </si>
+  <si>
+    <t>61bbe402-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>LastVisit</t>
+  </si>
+  <si>
+    <t>LastVisit &lt; RegistrationDate</t>
+  </si>
+  <si>
+    <t>Last visit date before registration date</t>
+  </si>
+  <si>
+    <t>61bc1d96-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>LastVisit IS NULL</t>
+  </si>
+  <si>
+    <t>LastVisit is Required</t>
+  </si>
+  <si>
+    <t>6c5c63e4-2a95-11e7-93ae-92361f002671</t>
+  </si>
+  <si>
+    <t>PatientID</t>
+  </si>
+  <si>
+    <t>PatientID IS NULL</t>
+  </si>
+  <si>
+    <t>PatientID Required</t>
+  </si>
+  <si>
+    <t>6c5c6100-2a95-11e7-93ae-92361f002671</t>
+  </si>
+  <si>
+    <t>PatientPK</t>
+  </si>
+  <si>
+    <t>PatientPK IS NULL</t>
+  </si>
+  <si>
+    <t>PatientPK Required</t>
+  </si>
+  <si>
+    <t>61bbefba-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>PreviousARTStartDate</t>
+  </si>
+  <si>
+    <t>PatientSource='Transfer-in' AND PreviousARTStartDate IS NULL</t>
+  </si>
+  <si>
+    <t>Transfer-in Patient missing Previous Start ART Date</t>
+  </si>
+  <si>
+    <t>61bc253e-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>PatientSource='Transfer-in' AND PreviousARTRegimen IS NULL</t>
+  </si>
+  <si>
+    <t>6c5c64fc-2a95-11e7-93ae-92361f002671</t>
+  </si>
+  <si>
+    <t>SiteCode</t>
+  </si>
+  <si>
+    <t>SiteCode IS NULL OR SiteCode = 0</t>
+  </si>
+  <si>
+    <t>SiteCode Required</t>
+  </si>
+  <si>
+    <t>ce7b5db8-160f-11e7-93ae-92361f002671</t>
+  </si>
+  <si>
+    <t>StartARTDate</t>
+  </si>
+  <si>
+    <t>StartARTDate IS NULL</t>
+  </si>
+  <si>
+    <t>StartARTDate Required</t>
+  </si>
+  <si>
+    <t>61bc1c9c-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>StartARTDate &gt; ExitDate</t>
+  </si>
+  <si>
+    <t>StartARTDate after Exit Date</t>
+  </si>
+  <si>
+    <t>61bc228c-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>StartARTDate&lt; 1997-01-01</t>
+  </si>
+  <si>
+    <t>StartARTDate out of expected range</t>
+  </si>
+  <si>
+    <t>61bc2372-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>StartARTDate &gt; LastVisit</t>
+  </si>
+  <si>
+    <t>StartARTDate after last visit date</t>
+  </si>
+  <si>
+    <t>61bc2624-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>StartARTDate=''</t>
+  </si>
+  <si>
+    <t>61bc2b92-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>StartARTDate &lt; RegistrationDate AND PatientSource &lt;&gt; 'Transfer In'</t>
+  </si>
+  <si>
+    <t>StartARTDate before patient registered</t>
+  </si>
+  <si>
+    <t>ce7b5f34-160f-11e7-93ae-92361f002671</t>
+  </si>
+  <si>
+    <t>StartRegimen</t>
+  </si>
+  <si>
+    <t>StartRegimen IS NULL</t>
+  </si>
+  <si>
+    <t>StartRegimen Required</t>
+  </si>
+  <si>
+    <t>61bbd7c8-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>StartRegimenLine</t>
+  </si>
+  <si>
+    <t>StartRegimenLine IS NULL</t>
+  </si>
+  <si>
+    <t>StartRegimenLine is Required</t>
+  </si>
+  <si>
+    <t>6c5c66fa-2a95-11e7-93ae-92361f002671</t>
+  </si>
+  <si>
+    <t>TempPatientBaselinesExtract</t>
+  </si>
+  <si>
+    <t>6c5c6600-2a95-11e7-93ae-92361f002671</t>
+  </si>
+  <si>
+    <t>6c5c6812-2a95-11e7-93ae-92361f002671</t>
+  </si>
+  <si>
+    <t>61bbd49e-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>TempPatientExtract</t>
+  </si>
+  <si>
+    <t>DOB &gt;= RegistrationAtCCC AND RegistrationAtCCC IS NOT Null</t>
+  </si>
+  <si>
+    <t>DoB After Date of Registration</t>
+  </si>
+  <si>
+    <t>ce7b5c1e-160f-11e7-93ae-92361f002671</t>
+  </si>
+  <si>
+    <t>DOB IS NULL</t>
+  </si>
+  <si>
+    <t>DOB Required</t>
+  </si>
+  <si>
     <t>ce7b571e-160f-11e7-93ae-92361f002671</t>
   </si>
   <si>
-    <t>TempPatientExtract</t>
-  </si>
-  <si>
     <t>Gender</t>
   </si>
   <si>
-    <t>Required</t>
-  </si>
-  <si>
     <t>Gender IS NULL</t>
   </si>
   <si>
     <t>Gender Required</t>
   </si>
   <si>
-    <t>ce7b5c1e-160f-11e7-93ae-92361f002671</t>
-  </si>
-  <si>
-    <t>DOB</t>
-  </si>
-  <si>
-    <t>DOB IS NULL</t>
-  </si>
-  <si>
-    <t>DOB Required</t>
-  </si>
-  <si>
-    <t>ce7b5db8-160f-11e7-93ae-92361f002671</t>
-  </si>
-  <si>
-    <t>TempPatientArtExtract</t>
-  </si>
-  <si>
-    <t>StartARTDate</t>
-  </si>
-  <si>
-    <t>StartARTDate IS NULL</t>
-  </si>
-  <si>
-    <t>StartARTDate Required</t>
-  </si>
-  <si>
-    <t>ce7b5f34-160f-11e7-93ae-92361f002671</t>
-  </si>
-  <si>
-    <t>StartRegimen</t>
-  </si>
-  <si>
-    <t>StartRegimen IS NULL</t>
-  </si>
-  <si>
-    <t>StartRegimen Required</t>
-  </si>
-  <si>
-    <t>6c5c6100-2a95-11e7-93ae-92361f002671</t>
-  </si>
-  <si>
-    <t>PatientPK</t>
-  </si>
-  <si>
-    <t>PatientPK IS NULL</t>
-  </si>
-  <si>
-    <t>PatientPK Required</t>
-  </si>
-  <si>
-    <t>6c5c63e4-2a95-11e7-93ae-92361f002671</t>
-  </si>
-  <si>
-    <t>PatientID</t>
-  </si>
-  <si>
-    <t>PatientID IS NULL</t>
-  </si>
-  <si>
-    <t>PatientID Required</t>
-  </si>
-  <si>
-    <t>6c5c64fc-2a95-11e7-93ae-92361f002671</t>
-  </si>
-  <si>
-    <t>SiteCode</t>
-  </si>
-  <si>
-    <t>SiteCode IS NULL</t>
-  </si>
-  <si>
-    <t>SiteCode Required</t>
-  </si>
-  <si>
-    <t>6c5c6600-2a95-11e7-93ae-92361f002671</t>
-  </si>
-  <si>
-    <t>TempPatientBaselinesExtract</t>
-  </si>
-  <si>
-    <t>6c5c66fa-2a95-11e7-93ae-92361f002671</t>
-  </si>
-  <si>
-    <t>6c5c6812-2a95-11e7-93ae-92361f002671</t>
+    <t>61bbe6d2-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>6c5c6c40-2a95-11e7-93ae-92361f002671</t>
   </si>
   <si>
     <t>6c5c6b28-2a95-11e7-93ae-92361f002671</t>
   </si>
   <si>
-    <t>6c5c6c40-2a95-11e7-93ae-92361f002671</t>
+    <t>61bc2f52-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>PatientSource</t>
+  </si>
+  <si>
+    <t>PatientSource IS NULL</t>
+  </si>
+  <si>
+    <t>PatientSource is required</t>
+  </si>
+  <si>
+    <t>61bbf186-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>RegistrationAtCCC</t>
+  </si>
+  <si>
+    <t>RegistrationAtCCC IS NULL</t>
+  </si>
+  <si>
+    <t>RegistrationAtCCC is Required</t>
   </si>
   <si>
     <t>6c5c70be-2a95-11e7-93ae-92361f002671</t>
   </si>
   <si>
+    <t>61bbedee-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>TempPatientLaboratoryExtract</t>
+  </si>
+  <si>
+    <t>OrderedByDate</t>
+  </si>
+  <si>
+    <t>OrderedByDate IS NULL</t>
+  </si>
+  <si>
+    <t>OrderedByDate is required</t>
+  </si>
+  <si>
+    <t>6c5c73e8-2a95-11e7-93ae-92361f002671</t>
+  </si>
+  <si>
     <t>6c5c72b2-2a95-11e7-93ae-92361f002671</t>
   </si>
   <si>
-    <t>TempPatientLaboratoryExtract</t>
-  </si>
-  <si>
-    <t>6c5c73e8-2a95-11e7-93ae-92361f002671</t>
-  </si>
-  <si>
     <t>6c5c780c-2a95-11e7-93ae-92361f002671</t>
   </si>
   <si>
+    <t>61bbeed4-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>TestName</t>
+  </si>
+  <si>
+    <t>TestName IS NULL</t>
+  </si>
+  <si>
+    <t>TestName is Required</t>
+  </si>
+  <si>
+    <t>61bbebc8-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>TempPatientPharmacyExtract</t>
+  </si>
+  <si>
+    <t>DispenseDate</t>
+  </si>
+  <si>
+    <t>DispenseDate IS NULL</t>
+  </si>
+  <si>
+    <t>DispenseDate is required</t>
+  </si>
+  <si>
+    <t>61bc2a52-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>Drug</t>
+  </si>
+  <si>
+    <t>Drug IS NULL</t>
+  </si>
+  <si>
+    <t>Drug Name is required</t>
+  </si>
+  <si>
+    <t>6c5c7a0a-2a95-11e7-93ae-92361f002671</t>
+  </si>
+  <si>
     <t>6c5c791a-2a95-11e7-93ae-92361f002671</t>
   </si>
   <si>
-    <t>TempPatientPharmacyExtract</t>
-  </si>
-  <si>
-    <t>6c5c7a0a-2a95-11e7-93ae-92361f002671</t>
-  </si>
-  <si>
     <t>6c5c7afa-2a95-11e7-93ae-92361f002671</t>
   </si>
   <si>
+    <t>61bc30ec-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>TempPatientStatusExtract</t>
+  </si>
+  <si>
+    <t>ExitDate</t>
+  </si>
+  <si>
+    <t>ExitDate IS NULL</t>
+  </si>
+  <si>
+    <t>ExitDate is required</t>
+  </si>
+  <si>
+    <t>61bc2458-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>61bc3204-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>ExitReason IS NULL</t>
+  </si>
+  <si>
+    <t>ExitReason is required</t>
+  </si>
+  <si>
+    <t>6c5c7cc6-2a95-11e7-93ae-92361f002671</t>
+  </si>
+  <si>
     <t>6c5c7bea-2a95-11e7-93ae-92361f002671</t>
   </si>
   <si>
-    <t>TempPatientStatusExtract</t>
-  </si>
-  <si>
-    <t>6c5c7cc6-2a95-11e7-93ae-92361f002671</t>
-  </si>
-  <si>
     <t>6c5c7db6-2a95-11e7-93ae-92361f002671</t>
   </si>
   <si>
+    <t>6c5c82d4-2a95-11e7-93ae-92361f002671</t>
+  </si>
+  <si>
+    <t>TempPatientVisitExtract</t>
+  </si>
+  <si>
     <t>6c5c81b2-2a95-11e7-93ae-92361f002671</t>
   </si>
   <si>
-    <t>TempPatientVisitExtract</t>
-  </si>
-  <si>
-    <t>6c5c82d4-2a95-11e7-93ae-92361f002671</t>
-  </si>
-  <si>
     <t>6c5c83b0-2a95-11e7-93ae-92361f002671</t>
+  </si>
+  <si>
+    <t>61bbe02e-35a1-11e7-a919-92ebcb67fe33</t>
+  </si>
+  <si>
+    <t>VisitDate</t>
+  </si>
+  <si>
+    <t>VisitDate IS NULL</t>
+  </si>
+  <si>
+    <t>VisitDate is required</t>
   </si>
 </sst>
 </file>
@@ -743,8 +1052,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F26" totalsRowShown="0">
-  <autoFilter ref="A1:F26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:F57" totalsRowShown="0">
+  <autoFilter ref="A1:F57"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Extract"/>
@@ -753,7 +1062,7 @@
     <tableColumn id="5" name="Logic"/>
     <tableColumn id="6" name="Summary"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1054,20 +1363,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection sqref="A1:F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1118,476 +1426,1096 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
       <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
         <v>39</v>
       </c>
-      <c r="B10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" t="s">
-        <v>31</v>
-      </c>
       <c r="F10" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="F11" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="F12" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E13" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="F13" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E14" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="F14" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="F15" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E16" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="F16" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="D17" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E17" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="F17" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="D18" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E18" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="F18" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="D19" t="s">
         <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="F19" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="D20" t="s">
         <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="F20" t="s">
-        <v>36</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="D21" t="s">
         <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="F21" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E22" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="F22" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="D23" t="s">
         <v>9</v>
       </c>
       <c r="E23" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="F23" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E24" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="F24" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="D25" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E25" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="F25" t="s">
-        <v>32</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>92</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
       <c r="C26" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="D26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B28" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" t="s">
         <v>9</v>
       </c>
-      <c r="E26" t="s">
-        <v>35</v>
-      </c>
-      <c r="F26" t="s">
-        <v>36</v>
+      <c r="E29" t="s">
+        <v>98</v>
+      </c>
+      <c r="F29" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" t="s">
+        <v>104</v>
+      </c>
+      <c r="D31" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" t="s">
+        <v>105</v>
+      </c>
+      <c r="F31" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>107</v>
+      </c>
+      <c r="B32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" t="s">
+        <v>46</v>
+      </c>
+      <c r="F32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" t="s">
+        <v>50</v>
+      </c>
+      <c r="F33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" t="s">
+        <v>30</v>
+      </c>
+      <c r="E34" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" t="s">
+        <v>111</v>
+      </c>
+      <c r="D35" t="s">
+        <v>30</v>
+      </c>
+      <c r="E35" t="s">
+        <v>112</v>
+      </c>
+      <c r="F35" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" t="s">
+        <v>115</v>
+      </c>
+      <c r="D36" t="s">
+        <v>30</v>
+      </c>
+      <c r="E36" t="s">
+        <v>116</v>
+      </c>
+      <c r="F36" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>118</v>
+      </c>
+      <c r="B37" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" t="s">
+        <v>30</v>
+      </c>
+      <c r="E37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>119</v>
+      </c>
+      <c r="B38" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" t="s">
+        <v>121</v>
+      </c>
+      <c r="D38" t="s">
+        <v>30</v>
+      </c>
+      <c r="E38" t="s">
+        <v>122</v>
+      </c>
+      <c r="F38" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>124</v>
+      </c>
+      <c r="B39" t="s">
+        <v>120</v>
+      </c>
+      <c r="C39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" t="s">
+        <v>30</v>
+      </c>
+      <c r="E39" t="s">
+        <v>50</v>
+      </c>
+      <c r="F39" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>125</v>
+      </c>
+      <c r="B40" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" t="s">
+        <v>54</v>
+      </c>
+      <c r="F40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>126</v>
+      </c>
+      <c r="B41" t="s">
+        <v>120</v>
+      </c>
+      <c r="C41" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F41" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>127</v>
+      </c>
+      <c r="B42" t="s">
+        <v>120</v>
+      </c>
+      <c r="C42" t="s">
+        <v>128</v>
+      </c>
+      <c r="D42" t="s">
+        <v>30</v>
+      </c>
+      <c r="E42" t="s">
+        <v>129</v>
+      </c>
+      <c r="F42" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" t="s">
+        <v>132</v>
+      </c>
+      <c r="C43" t="s">
+        <v>133</v>
+      </c>
+      <c r="D43" t="s">
+        <v>30</v>
+      </c>
+      <c r="E43" t="s">
+        <v>134</v>
+      </c>
+      <c r="F43" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>136</v>
+      </c>
+      <c r="B44" t="s">
+        <v>132</v>
+      </c>
+      <c r="C44" t="s">
+        <v>137</v>
+      </c>
+      <c r="D44" t="s">
+        <v>30</v>
+      </c>
+      <c r="E44" t="s">
+        <v>138</v>
+      </c>
+      <c r="F44" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>140</v>
+      </c>
+      <c r="B45" t="s">
+        <v>132</v>
+      </c>
+      <c r="C45" t="s">
+        <v>49</v>
+      </c>
+      <c r="D45" t="s">
+        <v>30</v>
+      </c>
+      <c r="E45" t="s">
+        <v>50</v>
+      </c>
+      <c r="F45" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>141</v>
+      </c>
+      <c r="B46" t="s">
+        <v>132</v>
+      </c>
+      <c r="C46" t="s">
+        <v>53</v>
+      </c>
+      <c r="D46" t="s">
+        <v>30</v>
+      </c>
+      <c r="E46" t="s">
+        <v>54</v>
+      </c>
+      <c r="F46" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>142</v>
+      </c>
+      <c r="B47" t="s">
+        <v>132</v>
+      </c>
+      <c r="C47" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E47" t="s">
+        <v>64</v>
+      </c>
+      <c r="F47" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>143</v>
+      </c>
+      <c r="B48" t="s">
+        <v>144</v>
+      </c>
+      <c r="C48" t="s">
+        <v>145</v>
+      </c>
+      <c r="D48" t="s">
+        <v>30</v>
+      </c>
+      <c r="E48" t="s">
+        <v>146</v>
+      </c>
+      <c r="F48" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>148</v>
+      </c>
+      <c r="B49" t="s">
+        <v>144</v>
+      </c>
+      <c r="C49" t="s">
+        <v>25</v>
+      </c>
+      <c r="D49" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" t="s">
+        <v>26</v>
+      </c>
+      <c r="F49" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>149</v>
+      </c>
+      <c r="B50" t="s">
+        <v>144</v>
+      </c>
+      <c r="C50" t="s">
+        <v>25</v>
+      </c>
+      <c r="D50" t="s">
+        <v>30</v>
+      </c>
+      <c r="E50" t="s">
+        <v>150</v>
+      </c>
+      <c r="F50" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>152</v>
+      </c>
+      <c r="B51" t="s">
+        <v>144</v>
+      </c>
+      <c r="C51" t="s">
+        <v>49</v>
+      </c>
+      <c r="D51" t="s">
+        <v>30</v>
+      </c>
+      <c r="E51" t="s">
+        <v>50</v>
+      </c>
+      <c r="F51" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>153</v>
+      </c>
+      <c r="B52" t="s">
+        <v>144</v>
+      </c>
+      <c r="C52" t="s">
+        <v>53</v>
+      </c>
+      <c r="D52" t="s">
+        <v>30</v>
+      </c>
+      <c r="E52" t="s">
+        <v>54</v>
+      </c>
+      <c r="F52" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>154</v>
+      </c>
+      <c r="B53" t="s">
+        <v>144</v>
+      </c>
+      <c r="C53" t="s">
+        <v>63</v>
+      </c>
+      <c r="D53" t="s">
+        <v>30</v>
+      </c>
+      <c r="E53" t="s">
+        <v>64</v>
+      </c>
+      <c r="F53" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>155</v>
+      </c>
+      <c r="B54" t="s">
+        <v>156</v>
+      </c>
+      <c r="C54" t="s">
+        <v>49</v>
+      </c>
+      <c r="D54" t="s">
+        <v>30</v>
+      </c>
+      <c r="E54" t="s">
+        <v>50</v>
+      </c>
+      <c r="F54" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>157</v>
+      </c>
+      <c r="B55" t="s">
+        <v>156</v>
+      </c>
+      <c r="C55" t="s">
+        <v>53</v>
+      </c>
+      <c r="D55" t="s">
+        <v>30</v>
+      </c>
+      <c r="E55" t="s">
+        <v>54</v>
+      </c>
+      <c r="F55" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>158</v>
+      </c>
+      <c r="B56" t="s">
+        <v>156</v>
+      </c>
+      <c r="C56" t="s">
+        <v>63</v>
+      </c>
+      <c r="D56" t="s">
+        <v>30</v>
+      </c>
+      <c r="E56" t="s">
+        <v>64</v>
+      </c>
+      <c r="F56" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>159</v>
+      </c>
+      <c r="B57" t="s">
+        <v>156</v>
+      </c>
+      <c r="C57" t="s">
+        <v>160</v>
+      </c>
+      <c r="D57" t="s">
+        <v>30</v>
+      </c>
+      <c r="E57" t="s">
+        <v>161</v>
+      </c>
+      <c r="F57" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>